<commit_message>
Editing Melanie's sulfide code to read in multiple plates
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/202511/Raw Data/20251114_COMPASS_H2S_Plate4.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/202511/Raw Data/20251114_COMPASS_H2S_Plate4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\microplate\Desktop\BioGeoChem_Microplates\COMPASS\H2S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5A9721-C476-473A-82C8-8D4B8876D8D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5835D530-99E6-418A-A676-CF6FD2AD0306}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="11640" xr2:uid="{B5C9614C-E24A-448B-8860-EC03100E88DC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="11640" xr2:uid="{77D8D9E1-1F09-4829-B78C-DF33517FD2EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +93,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -138,6 +144,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,12 +251,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.6809711286089242E-2"/>
-                  <c:y val="-1.7621755613881599E-3"/>
-                </c:manualLayout>
-              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -282,7 +283,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:f>Sheet1!$K$11:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -309,27 +310,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$16</c:f>
+              <c:f>Sheet1!$L$11:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.6000000000000003E-2</c:v>
+                  <c:v>6.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12066666666666666</c:v>
+                  <c:v>0.13066666666666668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22833333333333336</c:v>
+                  <c:v>0.25800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34266666666666667</c:v>
+                  <c:v>0.36233333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66899999999999993</c:v>
+                  <c:v>0.5645</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0083333333333333</c:v>
+                  <c:v>0.98066666666666658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,7 +338,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B4A9-40FB-B9FF-7EBA7B220609}"/>
+              <c16:uniqueId val="{00000000-70C3-407A-860D-F21FE46FF2E1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -349,11 +350,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="434005784"/>
-        <c:axId val="434008408"/>
+        <c:axId val="438148144"/>
+        <c:axId val="438146176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="434005784"/>
+        <c:axId val="438148144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,12 +411,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434008408"/>
+        <c:crossAx val="438146176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="434008408"/>
+        <c:axId val="438146176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,7 +473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434005784"/>
+        <c:crossAx val="438148144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1088,23 +1089,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F7D3A0D-AA5F-4A6F-85BE-1F207955939E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BCB7292-D543-4CC2-A509-1EB55CEF751F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1421,11 +1422,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3BCD68-93C2-4BDF-A87E-7FD9DEFC6CE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B12C6B-4F38-43F4-9E7F-C5B3BE0CBE86}">
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,40 +1475,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="C2" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E2" s="3">
-        <v>7.5999999999999998E-2</v>
+        <v>0.2</v>
       </c>
       <c r="F2" s="3">
-        <v>7.2999999999999995E-2</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="G2" s="3">
-        <v>7.6999999999999999E-2</v>
+        <v>0.187</v>
       </c>
       <c r="H2" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>0.747</v>
       </c>
       <c r="I2" s="3">
+        <v>0.751</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="K2" s="3">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="L2" s="3">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="J2" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="M2" s="3">
         <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="L2" s="3">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="M2" s="3">
-        <v>6.8000000000000005E-2</v>
       </c>
       <c r="N2" s="4">
         <v>670</v>
@@ -1518,40 +1519,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
+        <v>0.182</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.317</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.121</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="M3" s="3">
         <v>0.126</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.113</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.123</v>
-      </c>
-      <c r="E3" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>7.8E-2</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.08</v>
-      </c>
-      <c r="H3" s="3">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="I3" s="3">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="J3" s="3">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="K3" s="3">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="L3" s="3">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="M3" s="3">
-        <v>7.5999999999999998E-2</v>
       </c>
       <c r="N3" s="4">
         <v>670</v>
@@ -1562,40 +1563,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>0.252</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="C4" s="3">
-        <v>0.189</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="D4" s="3">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.317</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.224</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="M4" s="3">
         <v>0.24399999999999999</v>
-      </c>
-      <c r="E4" s="3">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="G4" s="3">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="I4" s="3">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="J4" s="3">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="K4" s="3">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.10199999999999999</v>
       </c>
       <c r="N4" s="4">
         <v>670</v>
@@ -1606,40 +1607,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>0.3</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="C5" s="3">
-        <v>0.308</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D5" s="3">
-        <v>0.42</v>
+        <v>0.35</v>
       </c>
       <c r="E5" s="3">
-        <v>7.1999999999999995E-2</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="F5" s="3">
-        <v>7.2999999999999995E-2</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G5" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="H5" s="3">
-        <v>6.9000000000000006E-2</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="I5" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="J5" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="K5" s="3">
-        <v>7.3999999999999996E-2</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="L5" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.376</v>
       </c>
       <c r="M5" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="N5" s="4">
         <v>670</v>
@@ -1650,40 +1651,40 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>0.63300000000000001</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="C6" s="3">
-        <v>0.64600000000000002</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="D6" s="3">
-        <v>0.72799999999999998</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="E6" s="3">
-        <v>6.2E-2</v>
+        <v>0.23</v>
       </c>
       <c r="F6" s="3">
-        <v>5.8999999999999997E-2</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="G6" s="3">
-        <v>0.06</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="H6" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>0.374</v>
       </c>
       <c r="I6" s="3">
-        <v>7.1999999999999995E-2</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="J6" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="K6" s="3">
-        <v>0.111</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="L6" s="3">
-        <v>0.108</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="M6" s="3">
-        <v>0.10199999999999999</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="N6" s="4">
         <v>670</v>
@@ -1694,40 +1695,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>1.04</v>
+        <v>1.163</v>
       </c>
       <c r="C7" s="3">
-        <v>0.98099999999999998</v>
+        <v>1.1479999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>1.004</v>
+        <v>1.0389999999999999</v>
       </c>
       <c r="E7" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="F7" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>0.497</v>
       </c>
       <c r="G7" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>0.496</v>
       </c>
       <c r="H7" s="3">
-        <v>7.1999999999999995E-2</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="I7" s="3">
-        <v>7.0999999999999994E-2</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="J7" s="3">
-        <v>6.9000000000000006E-2</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="K7" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="L7" s="3">
-        <v>7.3999999999999996E-2</v>
+        <v>0.97</v>
       </c>
       <c r="M7" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="N7" s="4">
         <v>670</v>
@@ -1738,40 +1739,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>1.232</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="C8" s="3">
-        <v>1.1060000000000001</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="D8" s="3">
-        <v>1.1140000000000001</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="E8" s="3">
-        <v>6.2E-2</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="F8" s="3">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="K8" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M8" s="3">
         <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="G8" s="3">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="I8" s="3">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="J8" s="3">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="L8" s="3">
-        <v>6.3E-2</v>
-      </c>
-      <c r="M8" s="3">
-        <v>5.8000000000000003E-2</v>
       </c>
       <c r="N8" s="4">
         <v>670</v>
@@ -1782,205 +1783,181 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>0.97</v>
+        <v>1.012</v>
       </c>
       <c r="C9" s="3">
-        <v>1.0449999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="3">
-        <v>1.2410000000000001</v>
+        <v>1.143</v>
       </c>
       <c r="E9" s="3">
-        <v>0.44400000000000001</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="F9" s="3">
-        <v>0.61499999999999999</v>
+        <v>1.121</v>
       </c>
       <c r="G9" s="3">
-        <v>0.60799999999999998</v>
+        <v>1.002</v>
       </c>
       <c r="H9" s="3">
-        <v>0.44700000000000001</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="I9" s="3">
-        <v>0.33700000000000002</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="J9" s="3">
-        <v>0.33700000000000002</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="K9" s="3">
-        <v>8.6999999999999994E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L9" s="3">
-        <v>0.1</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="M9" s="3">
-        <v>9.4E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="N9" s="4">
         <v>670</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <f>AVERAGE(B2:D2)</f>
-        <v>6.6000000000000003E-2</v>
-      </c>
       <c r="E11">
         <f>AVERAGE(E2:G2)</f>
-        <v>7.5333333333333322E-2</v>
+        <v>0.20600000000000004</v>
       </c>
       <c r="H11">
         <f>AVERAGE(H2:J2)</f>
-        <v>6.9666666666666668E-2</v>
+        <v>0.73999999999999988</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <f>AVERAGE(K2:M2)</f>
-        <v>6.8333333333333343E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="E12">
+        <f t="shared" ref="E12:E18" si="0">AVERAGE(E3:G3)</f>
+        <v>0.34333333333333332</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H18" si="1">AVERAGE(H3:J3)</f>
+        <v>0.71133333333333348</v>
+      </c>
+      <c r="K12">
         <v>5</v>
       </c>
-      <c r="B12">
-        <f t="shared" ref="B12:B18" si="0">AVERAGE(B3:D3)</f>
-        <v>0.12066666666666666</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E18" si="1">AVERAGE(E3:G3)</f>
-        <v>7.7666666666666662E-2</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ref="H12:H18" si="2">AVERAGE(H3:J3)</f>
-        <v>6.5666666666666665E-2</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ref="K12:K18" si="3">AVERAGE(K3:M3)</f>
-        <v>7.6666666666666661E-2</v>
+      <c r="L12">
+        <f t="shared" ref="L12:L18" si="2">AVERAGE(K3:M3)</f>
+        <v>0.13066666666666668</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.29033333333333333</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="K13">
         <v>12.5</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>0.22833333333333336</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>6.3333333333333339E-2</v>
-      </c>
-      <c r="H13">
+      <c r="L13">
         <f t="shared" si="2"/>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
-        <v>0.106</v>
+        <v>0.25800000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.48433333333333334</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.39666666666666667</v>
+      </c>
+      <c r="K14">
         <v>25</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>0.34266666666666667</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="H14">
+      <c r="L14">
         <f t="shared" si="2"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
-        <v>7.0666666666666669E-2</v>
+        <v>0.36233333333333334</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.21333333333333335</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.38366666666666666</v>
+      </c>
+      <c r="K15">
         <v>50</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0.66899999999999993</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>6.0333333333333329E-2</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>7.1333333333333318E-2</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="3"/>
-        <v>0.107</v>
+      <c r="L15">
+        <f>AVERAGE(L6:M6)</f>
+        <v>0.5645</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.52933333333333332</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.36766666666666664</v>
+      </c>
+      <c r="K16">
         <v>100</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1.0083333333333333</v>
-      </c>
-      <c r="E16">
+      <c r="L16" s="5">
+        <f t="shared" si="2"/>
+        <v>0.98066666666666658</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>AVERAGE(B8:D8)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E17" s="5">
+        <f>AVERAGE(E8:G8)</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
-        <v>6.533333333333334E-2</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>7.0666666666666669E-2</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="3"/>
-        <v>6.8000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1.1506666666666667</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="H17">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="2"/>
         <v>6.9333333333333344E-2</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
-        <v>6.0333333333333329E-2</v>
-      </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18">
+        <f>AVERAGE(B9:D9)</f>
+        <v>1.085</v>
+      </c>
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
-        <v>1.0853333333333333</v>
-      </c>
-      <c r="E18">
+        <v>1.0493333333333332</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="1"/>
-        <v>0.55566666666666664</v>
-      </c>
-      <c r="H18">
+        <v>0.6323333333333333</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="2"/>
-        <v>0.37366666666666665</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>9.3666666666666676E-2</v>
+        <v>6.7666666666666667E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>